<commit_message>
matriz en consulta 2 y join de las consultas base en consulta 4
</commit_message>
<xml_diff>
--- a/consulta2.xlsx
+++ b/consulta2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,79 +434,94 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Year</t>
+          <t>Eastern</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>RegionDescription</t>
+          <t>Northern</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>CompanyName</t>
+          <t>Southern</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>TotalCustomer</t>
+          <t>Westerns</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1998</v>
+        <v>1996</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Ernst Handel</t>
+        </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Eastern</t>
+          <t>Save-a-lot Markets</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>QUICK-Stop</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>22300</v>
+          <t>LILA-Supermercado</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Piccolo und mehr</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1998</v>
+        <v>1997</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>QUICK-Stop</t>
+        </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Northern</t>
+          <t>QUICK-Stop</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Rattlesnake Canyon Grocery</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>14364</v>
+          <t>QUICK-Stop</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Save-a-lot Markets</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>99</v>
-      </c>
-      <c r="B4" t="n">
         <v>1998</v>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>QUICK-Stop</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Southern</t>
+          <t>Rattlesnake Canyon Grocery</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -514,197 +529,10 @@
           <t>Hungry Owl All-Night Grocers</t>
         </is>
       </c>
-      <c r="E4" t="n">
-        <v>12280.74</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>129</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1998</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Westerns</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>Save-a-lot Markets</t>
         </is>
-      </c>
-      <c r="E5" t="n">
-        <v>23484.4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>164</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1997</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Eastern</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>QUICK-Stop</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>41337.5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>244</v>
-      </c>
-      <c r="B7" t="n">
-        <v>1997</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Northern</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>QUICK-Stop</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>9354.799999999999</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>286</v>
-      </c>
-      <c r="B8" t="n">
-        <v>1997</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Southern</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>QUICK-Stop</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>11875.7</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>332</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1997</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Westerns</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Save-a-lot Markets</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>16754.44</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>377</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1996</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Eastern</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Ernst Handel</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>12430.4</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>428</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1996</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Northern</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Save-a-lot Markets</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>6155.9</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>452</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1996</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Southern</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>LILA-Supermercado</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>3466.8</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>468</v>
-      </c>
-      <c r="B13" t="n">
-        <v>1996</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Westerns</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Piccolo und mehr</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>10741.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>